<commit_message>
se agrega una columna en el archivo de excel con el link para consulta rapida
</commit_message>
<xml_diff>
--- a/matriz_Scripts.xlsx
+++ b/matriz_Scripts.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Listados" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>id</t>
   </si>
@@ -79,13 +79,19 @@
   </si>
   <si>
     <t>Consulta los empleados que  estan activos en contratos y que no tengan foto en maestro de empleados</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>ver aqui</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +103,14 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -119,14 +133,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -439,19 +456,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="82.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,8 +486,11 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -484,8 +506,14 @@
       <c r="E2" t="s">
         <v>17</v>
       </c>
+      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">

</xml_diff>

<commit_message>
cargue scripts de datos falatantes kactus
</commit_message>
<xml_diff>
--- a/matriz_Scripts.xlsx
+++ b/matriz_Scripts.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Listados" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>id</t>
   </si>
@@ -85,6 +85,24 @@
   </si>
   <si>
     <t>ver aqui</t>
+  </si>
+  <si>
+    <t>DatosBaicos</t>
+  </si>
+  <si>
+    <t>Consulta los empleados que  estan activos en contratos y que no tengan los datos basicos completos</t>
+  </si>
+  <si>
+    <t>CasadoSinConyugue</t>
+  </si>
+  <si>
+    <t>Consulta los empleados que  estan activos en contratos y tienen marcado en biemple como casados pero no tiene conyugue registrado en bifamil</t>
+  </si>
+  <si>
+    <t>DatosLaborales</t>
+  </si>
+  <si>
+    <t>Consulta los empleados que  estan activos en contratos y tiene las referencias laborales incompletos</t>
   </si>
 </sst>
 </file>
@@ -456,16 +474,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="82.375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
   </cols>
@@ -510,9 +529,107 @@
         <v>19</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F4" r:id="rId2"/>
+    <hyperlink ref="F5" r:id="rId3"/>
+    <hyperlink ref="F3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>